<commit_message>
task 5 finished adding items from into the db
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmccloud-my.sharepoint.com/personal/puskar61_755421_pmc_edu_np/Documents/Desktop/intern/task 1 re/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk\OneDrive - Patan Multiple Campus\Desktop\intern\task 1 re\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,24 +24,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">code </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>price</t>
   </si>
   <si>
-    <t xml:space="preserve">translationcode </t>
-  </si>
-  <si>
-    <t>item1</t>
-  </si>
-  <si>
-    <t>item2</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>np</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>item4</t>
+  </si>
+  <si>
+    <t>item7</t>
+  </si>
+  <si>
+    <t>dance</t>
+  </si>
+  <si>
+    <t>nachh</t>
   </si>
 </sst>
 </file>
@@ -362,51 +374,51 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
         <v>20</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -415,6 +427,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0a16581e-e65d-4915-acde-fb50cc546b99" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B76367734C002498CEDD692F911DEDD" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="604d750f6bec0522e8816880bc61ffa3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0a16581e-e65d-4915-acde-fb50cc546b99" xmlns:ns4="269045e1-bb2b-4fa8-b6d4-f58fabc12ef1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="714184e53da7bf0a23052fbf202f4436" ns3:_="" ns4:_="">
     <xsd:import namespace="0a16581e-e65d-4915-acde-fb50cc546b99"/>
@@ -649,24 +678,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0a16581e-e65d-4915-acde-fb50cc546b99" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9123D2E-2B56-4C7A-8056-488D05B3D6AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="0a16581e-e65d-4915-acde-fb50cc546b99"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="269045e1-bb2b-4fa8-b6d4-f58fabc12ef1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A3D2947-0268-4970-B209-1FF5657426A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91D4B8ED-31E7-460F-8AD5-B0BEC62B6CBD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -683,29 +720,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A3D2947-0268-4970-B209-1FF5657426A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9123D2E-2B56-4C7A-8056-488D05B3D6AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0a16581e-e65d-4915-acde-fb50cc546b99"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="269045e1-bb2b-4fa8-b6d4-f58fabc12ef1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>